<commit_message>
Close row is empty
</commit_message>
<xml_diff>
--- a/public/template/Excel/template02.xlsx
+++ b/public/template/Excel/template02.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="1245" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="1245" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="情報" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="102">
   <si>
     <t>日付</t>
     <rPh sb="0" eb="2">
@@ -684,6 +684,15 @@
   <si>
     <t>910×910</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>910×911</t>
+  </si>
+  <si>
+    <t>910×912</t>
+  </si>
+  <si>
+    <t>910×913</t>
   </si>
 </sst>
 </file>
@@ -972,7 +981,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1237,6 +1246,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1297,6 +1309,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1317,15 +1338,6 @@
     </xf>
     <xf numFmtId="38" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1854,7 +1866,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1865,7 +1877,7 @@
   <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.4"/>
@@ -2056,8 +2068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2068,41 +2080,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="str">
+      <c r="A1" s="97" t="str">
         <f>IF(情報!A2="","",情報!A2)</f>
         <v>2018/11/13</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
     </row>
     <row r="2" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="97" t="str">
+      <c r="A2" s="98" t="str">
         <f>IF(情報!K2="","",情報!K2 &amp; "工場")</f>
         <v>千葉工場</v>
       </c>
-      <c r="B2" s="97"/>
+      <c r="B2" s="98"/>
       <c r="C2" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="98"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
@@ -2115,107 +2127,107 @@
       <c r="H4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="99" t="str">
+      <c r="I4" s="100" t="str">
         <f>IF(情報!U2="","",情報!U2 &amp; "　" &amp; 情報!V2)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="J4" s="99"/>
+      <c r="J4" s="100"/>
     </row>
     <row r="5" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
     </row>
     <row r="6" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="101" t="str">
+      <c r="B6" s="102" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　先行壁")</f>
         <v>門沢橋3丁目2048番・B号棟　先行壁</v>
       </c>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="102"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
     </row>
     <row r="7" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="103" t="str">
+      <c r="B7" s="104" t="str">
         <f>IF(情報!E2="","",情報!E2 &amp; "　" &amp; 情報!F2)</f>
         <v>211850　紅中㈱　多摩</v>
       </c>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="104"/>
-      <c r="H7" s="104"/>
-      <c r="I7" s="104"/>
-      <c r="J7" s="104"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="105"/>
+      <c r="J7" s="105"/>
     </row>
     <row r="8" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="105" t="str">
+      <c r="B8" s="106" t="str">
         <f>IF(情報!L2="","",情報!L2)</f>
         <v>2018/11/21</v>
       </c>
-      <c r="C8" s="106"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="106"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="107"/>
+      <c r="G8" s="107"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107"/>
+      <c r="J8" s="107"/>
     </row>
     <row r="9" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="103" t="str">
+      <c r="B9" s="104" t="str">
         <f>IF(情報!O2="","",情報!O2)</f>
         <v>海老名市門沢橋３丁目２−２１</v>
       </c>
-      <c r="C9" s="104"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="104"/>
-      <c r="F9" s="104"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="104"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
     </row>
     <row r="10" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="107"/>
-      <c r="C10" s="107"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="107"/>
-      <c r="I10" s="107"/>
-      <c r="J10" s="107"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="108"/>
+      <c r="G10" s="108"/>
+      <c r="H10" s="108"/>
+      <c r="I10" s="108"/>
+      <c r="J10" s="108"/>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2249,7 +2261,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>65</v>
       </c>
@@ -2276,69 +2288,108 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="6"/>
+    <row r="13" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="88" t="s">
+        <v>65</v>
+      </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="8"/>
+      <c r="C13" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>67</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="88" t="s">
+        <v>99</v>
+      </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="6"/>
+      <c r="I13" s="10">
+        <f t="shared" ref="I13:I15" si="0">SUM(G13:H13)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="88" t="s">
+        <v>65</v>
+      </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>67</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="88" t="s">
+        <v>100</v>
+      </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="6"/>
+      <c r="I14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="88" t="s">
+        <v>65</v>
+      </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="68" t="s">
+        <v>67</v>
+      </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="88" t="s">
+        <v>101</v>
+      </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="11"/>
+      <c r="I15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="69" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="90" t="s">
+      <c r="B16" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="93"/>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="89"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="94"/>
-      <c r="J17" s="95"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2365,7 +2416,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:J17"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2376,41 +2427,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="str">
+      <c r="A1" s="97" t="str">
         <f>IF(工場1便!A1="","",工場1便!A1)</f>
         <v>2018/11/13</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
     </row>
     <row r="2" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="97" t="str">
+      <c r="A2" s="98" t="str">
         <f>IF(工場1便!A2="","",工場1便!A2)</f>
         <v>千葉工場</v>
       </c>
-      <c r="B2" s="97"/>
+      <c r="B2" s="98"/>
       <c r="C2" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="98"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
     </row>
     <row r="4" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="84"/>
@@ -2423,108 +2474,108 @@
       <c r="H4" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="I4" s="99" t="str">
+      <c r="I4" s="100" t="str">
         <f>IF(工場1便!I4="","",工場1便!I4)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="J4" s="99"/>
+      <c r="J4" s="100"/>
     </row>
     <row r="5" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="101" t="str">
+      <c r="B6" s="102" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　天井")</f>
         <v>門沢橋3丁目2048番・B号棟　天井</v>
       </c>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="102"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
     </row>
     <row r="7" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="101" t="str">
+      <c r="B7" s="102" t="str">
         <f>IF(工場1便!B7="","",工場1便!B7)</f>
         <v>211850　紅中㈱　多摩</v>
       </c>
-      <c r="C7" s="102"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="102"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
       <c r="K7" s="15"/>
     </row>
     <row r="8" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="101" t="str">
+      <c r="B8" s="102" t="str">
         <f>IF(情報!M2="","",情報!M2)</f>
         <v>2018/11/30</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="101" t="str">
+      <c r="B9" s="102" t="str">
         <f>IF(工場1便!B9="","",工場1便!B9)</f>
         <v>海老名市門沢橋３丁目２−２１</v>
       </c>
-      <c r="C9" s="102"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="107"/>
-      <c r="C10" s="107"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="107"/>
-      <c r="I10" s="107"/>
-      <c r="J10" s="107"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="108"/>
+      <c r="G10" s="108"/>
+      <c r="H10" s="108"/>
+      <c r="I10" s="108"/>
+      <c r="J10" s="108"/>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2585,7 +2636,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>72</v>
       </c>
@@ -2612,7 +2663,7 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="87" t="s">
         <v>72</v>
       </c>
@@ -2639,7 +2690,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="87" t="s">
         <v>72</v>
       </c>
@@ -2667,47 +2718,47 @@
       <c r="L15" s="12"/>
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="90" t="s">
+      <c r="B16" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="93"/>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="89"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="94"/>
-      <c r="J17" s="95"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:J17"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2719,7 +2770,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2728,26 +2779,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="str">
+      <c r="A1" s="97" t="str">
         <f>IF(工場1便!A1="","",工場1便!A1)</f>
         <v>2018/11/13</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="97" t="str">
+      <c r="A2" s="98" t="str">
         <f>IF(工場1便!A2="","",工場1便!A2)</f>
         <v>千葉工場</v>
       </c>
-      <c r="B2" s="97"/>
+      <c r="B2" s="98"/>
       <c r="C2" s="1" t="s">
         <v>47</v>
       </c>
@@ -2760,16 +2811,16 @@
       <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="98"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
@@ -2782,108 +2833,108 @@
       <c r="H4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="99" t="str">
+      <c r="I4" s="100" t="str">
         <f>IF(工場1便!I4="","",工場1便!I4)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="J4" s="99"/>
+      <c r="J4" s="100"/>
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="101" t="str">
+      <c r="B6" s="102" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　壁")</f>
         <v>門沢橋3丁目2048番・B号棟　壁</v>
       </c>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="102"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
     </row>
     <row r="7" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="101" t="str">
+      <c r="B7" s="102" t="str">
         <f>IF(工場1便!B7="","",工場1便!B7)</f>
         <v>211850　紅中㈱　多摩</v>
       </c>
-      <c r="C7" s="102"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="102"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
       <c r="K7" s="15"/>
     </row>
     <row r="8" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="101" t="str">
+      <c r="B8" s="102" t="str">
         <f>IF(情報!N2="","",情報!N2)</f>
         <v>2018/11/30</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="101" t="str">
+      <c r="B9" s="102" t="str">
         <f>IF(工場1便!B9="","",工場1便!B9)</f>
         <v>海老名市門沢橋３丁目２−２１</v>
       </c>
-      <c r="C9" s="102"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="107"/>
-      <c r="C10" s="107"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="107"/>
-      <c r="I10" s="107"/>
-      <c r="J10" s="107"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="108"/>
+      <c r="G10" s="108"/>
+      <c r="H10" s="108"/>
+      <c r="I10" s="108"/>
+      <c r="J10" s="108"/>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2998,7 +3049,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" ht="12" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="87" t="s">
         <v>65</v>
       </c>
@@ -3026,47 +3077,47 @@
       <c r="L15" s="12"/>
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="90" t="s">
+      <c r="B16" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="93"/>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="89"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="94"/>
-      <c r="J17" s="95"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A5:J5"/>
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:J17"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A5:J5"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3078,7 +3129,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3096,89 +3147,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="96"/>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
+      <c r="A1" s="97"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="98"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
+      <c r="A2" s="99"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="96" t="str">
+      <c r="A3" s="97" t="str">
         <f>IF(情報!R2="","",情報!R2)</f>
         <v>東京都台東区寿3-14-11</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="96" t="str">
+      <c r="A4" s="97" t="str">
         <f>IF(情報!S2="","","TEL " &amp; 情報!S2)</f>
         <v>TEL 03-6635-1650</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="96" t="str">
+      <c r="A5" s="97" t="str">
         <f>IF(情報!T2="","","FAX " &amp; 情報!T2)</f>
         <v>FAX 03-5828-2860</v>
       </c>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="97"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="109"/>
+      <c r="B6" s="113"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
@@ -3189,36 +3240,36 @@
       <c r="J6" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="110" t="str">
+      <c r="K6" s="114" t="str">
         <f>IF(情報!U2="","",情報!U2 &amp; "　" &amp; 情報!V2)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="L6" s="110"/>
+      <c r="L6" s="114"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="111" t="str">
+      <c r="A7" s="115" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　先行壁")</f>
         <v>門沢橋3丁目2048番・B号棟　先行壁</v>
       </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
-      <c r="L7" s="111"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="115"/>
+      <c r="G7" s="115"/>
+      <c r="H7" s="115"/>
+      <c r="I7" s="115"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="115"/>
+      <c r="L7" s="115"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="108" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="107"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="19"/>
@@ -3294,7 +3345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="21" t="s">
         <v>65</v>
       </c>
@@ -3320,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="45" t="s">
         <v>65</v>
       </c>
@@ -3346,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="45" t="s">
         <v>65</v>
       </c>
@@ -3372,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="45" t="s">
         <v>65</v>
       </c>
@@ -3398,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="45" t="s">
         <v>65</v>
       </c>
@@ -3424,7 +3475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="45" t="s">
         <v>65</v>
       </c>
@@ -3451,34 +3502,34 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A17" s="112" t="s">
+      <c r="A17" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="112"/>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="113">
+      <c r="B17" s="116"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="117">
         <v>1</v>
       </c>
-      <c r="H17" s="113"/>
-      <c r="I17" s="113"/>
+      <c r="H17" s="117"/>
+      <c r="I17" s="117"/>
       <c r="J17" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="114"/>
-      <c r="L17" s="114"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="118"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A18" s="108" t="s">
+      <c r="A18" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="108"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
       <c r="G18" s="33">
         <v>74</v>
       </c>
@@ -3499,14 +3550,14 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A19" s="115" t="s">
+      <c r="A19" s="109" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="115"/>
-      <c r="C19" s="115"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="115"/>
-      <c r="F19" s="115"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="109"/>
       <c r="G19" s="32"/>
       <c r="H19" s="37"/>
       <c r="I19" s="37">
@@ -3515,18 +3566,18 @@
       <c r="J19" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="K19" s="116"/>
-      <c r="L19" s="116"/>
+      <c r="K19" s="110"/>
+      <c r="L19" s="110"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A20" s="115" t="s">
+      <c r="A20" s="109" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="115"/>
-      <c r="C20" s="115"/>
-      <c r="D20" s="115"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="115"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="109"/>
       <c r="G20" s="32"/>
       <c r="H20" s="37"/>
       <c r="I20" s="37">
@@ -3535,32 +3586,27 @@
       <c r="J20" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="K20" s="116"/>
-      <c r="L20" s="116"/>
+      <c r="K20" s="110"/>
+      <c r="L20" s="110"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A21" s="117" t="s">
+      <c r="A21" s="111" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="117"/>
-      <c r="C21" s="117"/>
-      <c r="D21" s="117"/>
-      <c r="E21" s="117"/>
-      <c r="F21" s="117"/>
-      <c r="G21" s="117"/>
-      <c r="H21" s="117"/>
-      <c r="I21" s="117"/>
-      <c r="J21" s="117"/>
-      <c r="K21" s="117"/>
-      <c r="L21" s="117"/>
+      <c r="B21" s="111"/>
+      <c r="C21" s="111"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="111"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
+      <c r="K21" s="111"/>
+      <c r="L21" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="A21:L21"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:L3"/>
@@ -3574,6 +3620,11 @@
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="K17:L17"/>
     <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="A21:L21"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3586,7 +3637,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -3604,89 +3655,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96"/>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
+      <c r="A1" s="97"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
     </row>
     <row r="2" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="98"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
+      <c r="A2" s="99"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
     </row>
     <row r="3" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="96" t="str">
+      <c r="A3" s="97" t="str">
         <f>IF(営業1便!A3="","",営業1便!A3)</f>
         <v>東京都台東区寿3-14-11</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
     </row>
     <row r="4" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="96" t="str">
+      <c r="A4" s="97" t="str">
         <f>IF(営業1便!A4="","",営業1便!A4)</f>
         <v>TEL 03-6635-1650</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
     </row>
     <row r="5" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="96" t="str">
+      <c r="A5" s="97" t="str">
         <f>IF(営業1便!A5="","",営業1便!A5)</f>
         <v>FAX 03-5828-2860</v>
       </c>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="97"/>
     </row>
     <row r="6" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="109"/>
+      <c r="B6" s="113"/>
       <c r="C6" s="71"/>
       <c r="D6" s="71"/>
       <c r="E6" s="71"/>
@@ -3697,36 +3748,36 @@
       <c r="J6" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="110" t="str">
+      <c r="K6" s="114" t="str">
         <f>IF(営業1便!K6="","",営業1便!K6)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="L6" s="110"/>
+      <c r="L6" s="114"/>
     </row>
     <row r="7" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="111" t="str">
+      <c r="A7" s="115" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　天井")</f>
         <v>門沢橋3丁目2048番・B号棟　天井</v>
       </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
-      <c r="L7" s="111"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="115"/>
+      <c r="G7" s="115"/>
+      <c r="H7" s="115"/>
+      <c r="I7" s="115"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="115"/>
+      <c r="L7" s="115"/>
     </row>
     <row r="8" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="108" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="107"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
       <c r="G8" s="64"/>
@@ -3830,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="66" t="s">
         <v>72</v>
       </c>
@@ -3856,7 +3907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="66" t="s">
         <v>72</v>
       </c>
@@ -3882,7 +3933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="66" t="s">
         <v>72</v>
       </c>
@@ -3908,7 +3959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="66" t="s">
         <v>72</v>
       </c>
@@ -3934,7 +3985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="66" t="s">
         <v>72</v>
       </c>
@@ -3961,34 +4012,34 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="112" t="s">
+      <c r="A17" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="112"/>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="113">
+      <c r="B17" s="116"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="117">
         <v>1</v>
       </c>
-      <c r="H17" s="113"/>
-      <c r="I17" s="113"/>
+      <c r="H17" s="117"/>
+      <c r="I17" s="117"/>
       <c r="J17" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="114"/>
-      <c r="L17" s="114"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="118"/>
     </row>
     <row r="18" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="108" t="s">
+      <c r="A18" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="108"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
       <c r="G18" s="78">
         <v>47</v>
       </c>
@@ -4009,14 +4060,14 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="115" t="s">
+      <c r="A19" s="109" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="115"/>
-      <c r="C19" s="115"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="115"/>
-      <c r="F19" s="115"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="109"/>
       <c r="G19" s="77"/>
       <c r="H19" s="82"/>
       <c r="I19" s="82">
@@ -4025,18 +4076,18 @@
       <c r="J19" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="K19" s="116"/>
-      <c r="L19" s="116"/>
+      <c r="K19" s="110"/>
+      <c r="L19" s="110"/>
     </row>
     <row r="20" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="115" t="s">
+      <c r="A20" s="109" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="115"/>
-      <c r="C20" s="115"/>
-      <c r="D20" s="115"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="115"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="109"/>
       <c r="G20" s="77"/>
       <c r="H20" s="82"/>
       <c r="I20" s="82">
@@ -4045,27 +4096,37 @@
       <c r="J20" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="K20" s="116"/>
-      <c r="L20" s="116"/>
+      <c r="K20" s="110"/>
+      <c r="L20" s="110"/>
     </row>
     <row r="21" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="117" t="s">
+      <c r="A21" s="111" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="117"/>
-      <c r="C21" s="117"/>
-      <c r="D21" s="117"/>
-      <c r="E21" s="117"/>
-      <c r="F21" s="117"/>
-      <c r="G21" s="117"/>
-      <c r="H21" s="117"/>
-      <c r="I21" s="117"/>
-      <c r="J21" s="117"/>
-      <c r="K21" s="117"/>
-      <c r="L21" s="117"/>
+      <c r="B21" s="111"/>
+      <c r="C21" s="111"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="111"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
+      <c r="K21" s="111"/>
+      <c r="L21" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="A21:L21"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="K6:L6"/>
@@ -4074,16 +4135,6 @@
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="K17:L17"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A5:L5"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4095,8 +4146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4112,101 +4163,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
       <c r="M1" s="39"/>
       <c r="N1" s="39"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A2" s="98"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
+      <c r="A2" s="99"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
       <c r="M2" s="41"/>
       <c r="N2" s="41"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A3" s="96" t="str">
+      <c r="A3" s="97" t="str">
         <f>IF(営業1便!A3="","",営業1便!A3)</f>
         <v>東京都台東区寿3-14-11</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
       <c r="M3" s="39"/>
       <c r="N3" s="39"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="96" t="str">
+      <c r="A4" s="97" t="str">
         <f>IF(営業1便!A4="","",営業1便!A4)</f>
         <v>TEL 03-6635-1650</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
       <c r="M4" s="39"/>
       <c r="N4" s="39"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A5" s="96" t="str">
+      <c r="A5" s="97" t="str">
         <f>IF(営業1便!A5="","",営業1便!A5)</f>
         <v>FAX 03-5828-2860</v>
       </c>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="97"/>
       <c r="M5" s="39"/>
       <c r="N5" s="39"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="109"/>
+      <c r="B6" s="113"/>
       <c r="C6" s="50"/>
       <c r="D6" s="50"/>
       <c r="E6" s="50"/>
@@ -4217,40 +4268,40 @@
       <c r="J6" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="110" t="str">
+      <c r="K6" s="114" t="str">
         <f>IF(営業1便!K6="","",営業1便!K6)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="L6" s="110"/>
+      <c r="L6" s="114"/>
       <c r="M6" s="41"/>
       <c r="N6" s="41"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A7" s="111" t="str">
+      <c r="A7" s="115" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　壁")</f>
         <v>門沢橋3丁目2048番・B号棟　壁</v>
       </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
-      <c r="L7" s="111"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="115"/>
+      <c r="G7" s="115"/>
+      <c r="H7" s="115"/>
+      <c r="I7" s="115"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="115"/>
+      <c r="L7" s="115"/>
       <c r="M7" s="40"/>
       <c r="N7" s="40"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="108" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="107"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
       <c r="G8" s="43"/>
@@ -4448,7 +4499,7 @@
       <c r="M14" s="41"/>
       <c r="N14" s="41"/>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="66" t="s">
         <v>65</v>
       </c>
@@ -4476,7 +4527,7 @@
       <c r="M15" s="41"/>
       <c r="N15" s="41"/>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="66" t="s">
         <v>65</v>
       </c>
@@ -4505,36 +4556,36 @@
       <c r="N16" s="41"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A17" s="112" t="s">
+      <c r="A17" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="112"/>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="113">
+      <c r="B17" s="116"/>
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="117">
         <v>1</v>
       </c>
-      <c r="H17" s="113"/>
-      <c r="I17" s="113"/>
+      <c r="H17" s="117"/>
+      <c r="I17" s="117"/>
       <c r="J17" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="114"/>
-      <c r="L17" s="114"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="118"/>
       <c r="M17" s="41"/>
       <c r="N17" s="41"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A18" s="108" t="s">
+      <c r="A18" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="108"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
       <c r="G18" s="57">
         <v>264</v>
       </c>
@@ -4557,14 +4608,14 @@
       <c r="N18" s="41"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A19" s="115" t="s">
+      <c r="A19" s="109" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="115"/>
-      <c r="C19" s="115"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="115"/>
-      <c r="F19" s="115"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="109"/>
       <c r="G19" s="56"/>
       <c r="H19" s="61"/>
       <c r="I19" s="61">
@@ -4573,20 +4624,20 @@
       <c r="J19" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="K19" s="116"/>
-      <c r="L19" s="116"/>
+      <c r="K19" s="110"/>
+      <c r="L19" s="110"/>
       <c r="M19" s="41"/>
       <c r="N19" s="41"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A20" s="115" t="s">
+      <c r="A20" s="109" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="115"/>
-      <c r="C20" s="115"/>
-      <c r="D20" s="115"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="115"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="109"/>
       <c r="G20" s="56"/>
       <c r="H20" s="61"/>
       <c r="I20" s="61">
@@ -4595,26 +4646,26 @@
       <c r="J20" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="K20" s="116"/>
-      <c r="L20" s="116"/>
+      <c r="K20" s="110"/>
+      <c r="L20" s="110"/>
       <c r="M20" s="41"/>
       <c r="N20" s="41"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A21" s="117" t="s">
+      <c r="A21" s="111" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="117"/>
-      <c r="C21" s="117"/>
-      <c r="D21" s="117"/>
-      <c r="E21" s="117"/>
-      <c r="F21" s="117"/>
-      <c r="G21" s="117"/>
-      <c r="H21" s="117"/>
-      <c r="I21" s="117"/>
-      <c r="J21" s="117"/>
-      <c r="K21" s="117"/>
-      <c r="L21" s="117"/>
+      <c r="B21" s="111"/>
+      <c r="C21" s="111"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="111"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
+      <c r="K21" s="111"/>
+      <c r="L21" s="111"/>
       <c r="M21" s="41"/>
       <c r="N21" s="41"/>
     </row>
@@ -4652,6 +4703,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="K17:L17"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="A1:L1"/>
@@ -4659,17 +4721,6 @@
     <mergeCell ref="A3:L3"/>
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="A21:L21"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update file pdf 7
</commit_message>
<xml_diff>
--- a/public/template/Excel/template02.xlsx
+++ b/public/template/Excel/template02.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\moudle03\public\template\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="1245" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="1245" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="情報" sheetId="1" r:id="rId1"/>
@@ -15,12 +20,12 @@
     <sheet name="営業2便" sheetId="5" r:id="rId6"/>
     <sheet name="営業3便" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="105">
   <si>
     <t>日付</t>
     <rPh sb="0" eb="2">
@@ -686,13 +691,28 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>910×911</t>
-  </si>
-  <si>
-    <t>910×912</t>
-  </si>
-  <si>
-    <t>910×913</t>
+    <t>910×910</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>910×910</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>910×1820</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>910×1820</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>910×1820</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>910×1820</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -1353,6 +1373,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1866,7 +1889,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2066,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2326,7 +2349,7 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="88" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -2351,7 +2374,7 @@
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="88" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -2415,7 +2438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -2771,7 +2794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -3124,6 +3147,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3131,7 +3155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
@@ -3633,8 +3657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -3857,7 +3881,7 @@
       </c>
       <c r="E11" s="66"/>
       <c r="F11" s="86" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="G11" s="77"/>
       <c r="H11" s="78"/>
@@ -3884,7 +3908,9 @@
         <v>67</v>
       </c>
       <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
+      <c r="F12" s="66" t="s">
+        <v>102</v>
+      </c>
       <c r="G12" s="78"/>
       <c r="H12" s="78"/>
       <c r="I12" s="79">
@@ -3910,7 +3936,9 @@
         <v>67</v>
       </c>
       <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
+      <c r="F13" s="66" t="s">
+        <v>103</v>
+      </c>
       <c r="G13" s="77"/>
       <c r="H13" s="78"/>
       <c r="I13" s="79">
@@ -3936,7 +3964,9 @@
         <v>67</v>
       </c>
       <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
+      <c r="F14" s="66" t="s">
+        <v>102</v>
+      </c>
       <c r="G14" s="78"/>
       <c r="H14" s="78"/>
       <c r="I14" s="79">
@@ -3962,7 +3992,9 @@
         <v>67</v>
       </c>
       <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
+      <c r="F15" s="66" t="s">
+        <v>104</v>
+      </c>
       <c r="G15" s="78"/>
       <c r="H15" s="78"/>
       <c r="I15" s="79">
@@ -3988,7 +4020,9 @@
         <v>67</v>
       </c>
       <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
+      <c r="F16" s="66" t="s">
+        <v>103</v>
+      </c>
       <c r="G16" s="78"/>
       <c r="H16" s="78"/>
       <c r="I16" s="79">
@@ -4131,7 +4165,8 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4139,7 +4174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update template file excel
</commit_message>
<xml_diff>
--- a/public/template/Excel/template02.xlsx
+++ b/public/template/Excel/template02.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TrungNV\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Module03\public\template\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2096555-4FA6-46B3-ABB1-A46D59F8C46A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E197D5D9-ECBF-414B-922C-D53E0AD860D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="1245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -994,7 +994,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1262,6 +1262,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1322,6 +1325,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1342,15 +1354,6 @@
     </xf>
     <xf numFmtId="38" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1654,7 +1657,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1706,7 +1709,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2114,41 +2117,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="97" t="str">
+      <c r="A1" s="98" t="str">
         <f>IF(情報!A2="","",情報!A2)</f>
         <v>2018/11/13</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
     </row>
     <row r="2" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="98" t="str">
+      <c r="A2" s="99" t="str">
         <f>IF(情報!K2="","",情報!K2 &amp; "工場")</f>
         <v>千葉工場</v>
       </c>
-      <c r="B2" s="98"/>
+      <c r="B2" s="99"/>
       <c r="C2" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="99"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
@@ -2161,107 +2164,107 @@
       <c r="H4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="100" t="str">
+      <c r="I4" s="101" t="str">
         <f>IF(情報!U2="","",情報!U2 &amp; "　" &amp; 情報!V2)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="J4" s="100"/>
+      <c r="J4" s="101"/>
     </row>
     <row r="5" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="101"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
     </row>
     <row r="6" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="102" t="str">
+      <c r="B6" s="103" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　先行壁")</f>
         <v>門沢橋3丁目2048番・B号棟　先行壁</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
     </row>
     <row r="7" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="104" t="str">
+      <c r="B7" s="105" t="str">
         <f>IF(情報!E2="","",情報!E2 &amp; "　" &amp; 情報!F2)</f>
         <v>211850　紅中㈱　多摩</v>
       </c>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="105"/>
-      <c r="I7" s="105"/>
-      <c r="J7" s="105"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
     </row>
     <row r="8" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="106" t="str">
+      <c r="B8" s="107" t="str">
         <f>IF(情報!L2="","",情報!L2)</f>
         <v>2018/11/21</v>
       </c>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
+      <c r="G8" s="108"/>
+      <c r="H8" s="108"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="108"/>
     </row>
     <row r="9" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="104" t="str">
+      <c r="B9" s="105" t="str">
         <f>IF(情報!O2="","",情報!O2)</f>
         <v>海老名市門沢橋３丁目２−２１</v>
       </c>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="105"/>
-      <c r="H9" s="105"/>
-      <c r="I9" s="105"/>
-      <c r="J9" s="105"/>
+      <c r="C9" s="106"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="106"/>
+      <c r="F9" s="106"/>
+      <c r="G9" s="106"/>
+      <c r="H9" s="106"/>
+      <c r="I9" s="106"/>
+      <c r="J9" s="106"/>
     </row>
     <row r="10" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="108"/>
-      <c r="G10" s="108"/>
-      <c r="H10" s="108"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="108"/>
+      <c r="B10" s="109"/>
+      <c r="C10" s="109"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="109"/>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2398,32 +2401,32 @@
       </c>
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="89" t="s">
+      <c r="A16" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="93"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="94"/>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="90"/>
-      <c r="B17" s="94"/>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="96"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2463,41 +2466,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="97" t="str">
+      <c r="A1" s="98" t="str">
         <f>IF(工場1便!A1="","",工場1便!A1)</f>
         <v>2018/11/13</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
     </row>
     <row r="2" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="98" t="str">
+      <c r="A2" s="99" t="str">
         <f>IF(工場1便!A2="","",工場1便!A2)</f>
         <v>千葉工場</v>
       </c>
-      <c r="B2" s="98"/>
+      <c r="B2" s="99"/>
       <c r="C2" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="99"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
     </row>
     <row r="4" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="84"/>
@@ -2510,108 +2513,108 @@
       <c r="H4" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="I4" s="100" t="str">
+      <c r="I4" s="101" t="str">
         <f>IF(工場1便!I4="","",工場1便!I4)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="J4" s="100"/>
+      <c r="J4" s="101"/>
     </row>
     <row r="5" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="101"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="102" t="str">
+      <c r="B6" s="103" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　天井")</f>
         <v>門沢橋3丁目2048番・B号棟　天井</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
     </row>
     <row r="7" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="102" t="str">
+      <c r="B7" s="103" t="str">
         <f>IF(工場1便!B7="","",工場1便!B7)</f>
         <v>211850　紅中㈱　多摩</v>
       </c>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="104"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="104"/>
       <c r="K7" s="15"/>
     </row>
     <row r="8" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="102" t="str">
+      <c r="B8" s="103" t="str">
         <f>IF(情報!M2="","",情報!M2)</f>
         <v>2018/11/30</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="104"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="102" t="str">
+      <c r="B9" s="103" t="str">
         <f>IF(工場1便!B9="","",工場1便!B9)</f>
         <v>海老名市門沢橋３丁目２−２１</v>
       </c>
-      <c r="C9" s="103"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="103"/>
-      <c r="F9" s="103"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="103"/>
-      <c r="J9" s="103"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="108"/>
-      <c r="G10" s="108"/>
-      <c r="H10" s="108"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="108"/>
+      <c r="B10" s="109"/>
+      <c r="C10" s="109"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="109"/>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -2754,47 +2757,47 @@
       <c r="L15" s="12"/>
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="89" t="s">
+      <c r="A16" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="93"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="94"/>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="90"/>
-      <c r="B17" s="94"/>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="96"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:J17"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2816,26 +2819,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="97" t="str">
+      <c r="A1" s="98" t="str">
         <f>IF(工場1便!A1="","",工場1便!A1)</f>
         <v>2018/11/13</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="98" t="str">
+      <c r="A2" s="99" t="str">
         <f>IF(工場1便!A2="","",工場1便!A2)</f>
         <v>千葉工場</v>
       </c>
-      <c r="B2" s="98"/>
+      <c r="B2" s="99"/>
       <c r="C2" s="1" t="s">
         <v>47</v>
       </c>
@@ -2848,16 +2851,16 @@
       <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="99"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
@@ -2870,108 +2873,108 @@
       <c r="H4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="100" t="str">
+      <c r="I4" s="101" t="str">
         <f>IF(工場1便!I4="","",工場1便!I4)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="J4" s="100"/>
+      <c r="J4" s="101"/>
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="101"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="101"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="102" t="str">
+      <c r="B6" s="103" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　壁")</f>
         <v>門沢橋3丁目2048番・B号棟　壁</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
     </row>
     <row r="7" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="102" t="str">
+      <c r="B7" s="103" t="str">
         <f>IF(工場1便!B7="","",工場1便!B7)</f>
         <v>211850　紅中㈱　多摩</v>
       </c>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="104"/>
+      <c r="I7" s="104"/>
+      <c r="J7" s="104"/>
       <c r="K7" s="15"/>
     </row>
     <row r="8" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="102" t="str">
+      <c r="B8" s="103" t="str">
         <f>IF(情報!N2="","",情報!N2)</f>
         <v>2018/11/30</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="104"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="102" t="str">
+      <c r="B9" s="103" t="str">
         <f>IF(工場1便!B9="","",工場1便!B9)</f>
         <v>海老名市門沢橋３丁目２−２１</v>
       </c>
-      <c r="C9" s="103"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="103"/>
-      <c r="F9" s="103"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="103"/>
-      <c r="J9" s="103"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="108"/>
-      <c r="F10" s="108"/>
-      <c r="G10" s="108"/>
-      <c r="H10" s="108"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="108"/>
+      <c r="B10" s="109"/>
+      <c r="C10" s="109"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="109"/>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
@@ -3114,47 +3117,47 @@
       <c r="L15" s="12"/>
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="89" t="s">
+      <c r="A16" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="93"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="93"/>
+      <c r="J16" s="94"/>
     </row>
     <row r="17" spans="1:10" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="90"/>
-      <c r="B17" s="94"/>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="96"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A5:J5"/>
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:J17"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A5:J5"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3165,8 +3168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -3178,89 +3181,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="97"/>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
+      <c r="A1" s="98"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
     </row>
     <row r="2" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
     </row>
     <row r="3" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="97" t="str">
+      <c r="A3" s="98" t="str">
         <f>IF(情報!R2="","",情報!R2)</f>
         <v>東京都台東区寿3-14-11</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
     </row>
     <row r="4" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="97" t="str">
+      <c r="A4" s="98" t="str">
         <f>IF(情報!S2="","","TEL " &amp; 情報!S2)</f>
         <v>TEL 03-6635-1650</v>
       </c>
-      <c r="B4" s="97"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
     </row>
     <row r="5" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="97" t="str">
+      <c r="A5" s="98" t="str">
         <f>IF(情報!T2="","","FAX " &amp; 情報!T2)</f>
         <v>FAX 03-5828-2860</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
     </row>
     <row r="6" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="110"/>
+      <c r="B6" s="114"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
@@ -3271,36 +3274,36 @@
       <c r="J6" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="111" t="str">
+      <c r="K6" s="115" t="str">
         <f>IF(情報!U2="","",情報!U2 &amp; "　" &amp; 情報!V2)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="L6" s="111"/>
+      <c r="L6" s="115"/>
     </row>
     <row r="7" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="112" t="str">
+      <c r="A7" s="116" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　先行壁")</f>
         <v>門沢橋3丁目2048番・B号棟　先行壁</v>
       </c>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="116"/>
+      <c r="L7" s="116"/>
     </row>
     <row r="8" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="108" t="s">
+      <c r="A8" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="109"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="19"/>
@@ -3533,43 +3536,45 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="113" t="s">
+      <c r="A17" s="117" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="113"/>
-      <c r="C17" s="113"/>
-      <c r="D17" s="113"/>
-      <c r="E17" s="113"/>
-      <c r="F17" s="113"/>
-      <c r="G17" s="114">
+      <c r="B17" s="117"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="118">
         <v>1</v>
       </c>
-      <c r="H17" s="114"/>
-      <c r="I17" s="114"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="118"/>
       <c r="J17" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="115"/>
-      <c r="L17" s="115"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
     </row>
     <row r="18" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="109" t="s">
+      <c r="A18" s="113" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="109"/>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
-      <c r="G18" s="33">
-        <v>74</v>
-      </c>
-      <c r="H18" s="33">
-        <v>99</v>
+      <c r="B18" s="113"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="89" t="str">
+        <f>IF(情報!B12="","",情報!B12)</f>
+        <v/>
+      </c>
+      <c r="H18" s="89" t="str">
+        <f>IF(情報!C12="","",情報!C12)</f>
+        <v/>
       </c>
       <c r="I18" s="34">
         <f>SUM(G18:H18)</f>
-        <v>173</v>
+        <v>0</v>
       </c>
       <c r="J18" s="24" t="s">
         <v>89</v>
@@ -3581,14 +3586,14 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="116" t="s">
+      <c r="A19" s="110" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="116"/>
-      <c r="F19" s="116"/>
+      <c r="B19" s="110"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="110"/>
       <c r="G19" s="32"/>
       <c r="H19" s="37"/>
       <c r="I19" s="37">
@@ -3597,18 +3602,18 @@
       <c r="J19" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="K19" s="117"/>
-      <c r="L19" s="117"/>
+      <c r="K19" s="111"/>
+      <c r="L19" s="111"/>
     </row>
     <row r="20" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="116" t="s">
+      <c r="A20" s="110" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="116"/>
-      <c r="F20" s="116"/>
+      <c r="B20" s="110"/>
+      <c r="C20" s="110"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="110"/>
       <c r="G20" s="32"/>
       <c r="H20" s="37"/>
       <c r="I20" s="37">
@@ -3617,32 +3622,27 @@
       <c r="J20" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="K20" s="117"/>
-      <c r="L20" s="117"/>
+      <c r="K20" s="111"/>
+      <c r="L20" s="111"/>
     </row>
     <row r="21" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="118" t="s">
+      <c r="A21" s="112" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="118"/>
-      <c r="K21" s="118"/>
-      <c r="L21" s="118"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="112"/>
+      <c r="L21" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="A21:L21"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:L3"/>
@@ -3656,6 +3656,11 @@
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="K17:L17"/>
     <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="A21:L21"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3667,8 +3672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -3682,89 +3687,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="97"/>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
+      <c r="A1" s="98"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
     </row>
     <row r="2" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
     </row>
     <row r="3" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="97" t="str">
+      <c r="A3" s="98" t="str">
         <f>IF(営業1便!A3="","",営業1便!A3)</f>
         <v>東京都台東区寿3-14-11</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
     </row>
     <row r="4" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="97" t="str">
+      <c r="A4" s="98" t="str">
         <f>IF(営業1便!A4="","",営業1便!A4)</f>
         <v>TEL 03-6635-1650</v>
       </c>
-      <c r="B4" s="97"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
     </row>
     <row r="5" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="97" t="str">
+      <c r="A5" s="98" t="str">
         <f>IF(営業1便!A5="","",営業1便!A5)</f>
         <v>FAX 03-5828-2860</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
     </row>
     <row r="6" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="110"/>
+      <c r="B6" s="114"/>
       <c r="C6" s="71"/>
       <c r="D6" s="71"/>
       <c r="E6" s="71"/>
@@ -3775,36 +3780,36 @@
       <c r="J6" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="111" t="str">
+      <c r="K6" s="115" t="str">
         <f>IF(営業1便!K6="","",営業1便!K6)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="L6" s="111"/>
+      <c r="L6" s="115"/>
     </row>
     <row r="7" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="112" t="str">
+      <c r="A7" s="116" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　天井")</f>
         <v>門沢橋3丁目2048番・B号棟　天井</v>
       </c>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="116"/>
+      <c r="L7" s="116"/>
     </row>
     <row r="8" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="108" t="s">
+      <c r="A8" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="109"/>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
       <c r="G8" s="64"/>
@@ -4039,43 +4044,45 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="113" t="s">
+      <c r="A17" s="117" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="113"/>
-      <c r="C17" s="113"/>
-      <c r="D17" s="113"/>
-      <c r="E17" s="113"/>
-      <c r="F17" s="113"/>
-      <c r="G17" s="114">
+      <c r="B17" s="117"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="118">
         <v>1</v>
       </c>
-      <c r="H17" s="114"/>
-      <c r="I17" s="114"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="118"/>
       <c r="J17" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="115"/>
-      <c r="L17" s="115"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
     </row>
     <row r="18" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="109" t="s">
+      <c r="A18" s="113" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="109"/>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
-      <c r="G18" s="78">
-        <v>47</v>
-      </c>
-      <c r="H18" s="78">
-        <v>48</v>
+      <c r="B18" s="113"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="89" t="str">
+        <f>IF(情報!B13="","",情報!B13)</f>
+        <v/>
+      </c>
+      <c r="H18" s="89" t="str">
+        <f>IF(情報!C13="","",情報!C13)</f>
+        <v/>
       </c>
       <c r="I18" s="79">
         <f>SUM(G18:H18)</f>
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="J18" s="69" t="s">
         <v>89</v>
@@ -4087,14 +4094,14 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="116" t="s">
+      <c r="A19" s="110" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="116"/>
-      <c r="F19" s="116"/>
+      <c r="B19" s="110"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="110"/>
       <c r="G19" s="77"/>
       <c r="H19" s="82"/>
       <c r="I19" s="82">
@@ -4103,18 +4110,18 @@
       <c r="J19" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="K19" s="117"/>
-      <c r="L19" s="117"/>
+      <c r="K19" s="111"/>
+      <c r="L19" s="111"/>
     </row>
     <row r="20" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="116" t="s">
+      <c r="A20" s="110" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="116"/>
-      <c r="F20" s="116"/>
+      <c r="B20" s="110"/>
+      <c r="C20" s="110"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="110"/>
       <c r="G20" s="77"/>
       <c r="H20" s="82"/>
       <c r="I20" s="82">
@@ -4123,27 +4130,37 @@
       <c r="J20" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="K20" s="117"/>
-      <c r="L20" s="117"/>
+      <c r="K20" s="111"/>
+      <c r="L20" s="111"/>
     </row>
     <row r="21" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="118" t="s">
+      <c r="A21" s="112" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="118"/>
-      <c r="K21" s="118"/>
-      <c r="L21" s="118"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="112"/>
+      <c r="L21" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="A21:L21"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="K6:L6"/>
@@ -4152,16 +4169,6 @@
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="K17:L17"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A5:L5"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4173,8 +4180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -4185,101 +4192,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="98" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
       <c r="M1" s="39"/>
       <c r="N1" s="39"/>
     </row>
     <row r="2" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
       <c r="M2" s="41"/>
       <c r="N2" s="41"/>
     </row>
     <row r="3" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="97" t="str">
+      <c r="A3" s="98" t="str">
         <f>IF(営業1便!A3="","",営業1便!A3)</f>
         <v>東京都台東区寿3-14-11</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
       <c r="M3" s="39"/>
       <c r="N3" s="39"/>
     </row>
     <row r="4" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="97" t="str">
+      <c r="A4" s="98" t="str">
         <f>IF(営業1便!A4="","",営業1便!A4)</f>
         <v>TEL 03-6635-1650</v>
       </c>
-      <c r="B4" s="97"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
       <c r="M4" s="39"/>
       <c r="N4" s="39"/>
     </row>
     <row r="5" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="97" t="str">
+      <c r="A5" s="98" t="str">
         <f>IF(営業1便!A5="","",営業1便!A5)</f>
         <v>FAX 03-5828-2860</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
       <c r="M5" s="39"/>
       <c r="N5" s="39"/>
     </row>
     <row r="6" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="110"/>
+      <c r="B6" s="114"/>
       <c r="C6" s="50"/>
       <c r="D6" s="50"/>
       <c r="E6" s="50"/>
@@ -4290,40 +4297,40 @@
       <c r="J6" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="111" t="str">
+      <c r="K6" s="115" t="str">
         <f>IF(営業1便!K6="","",営業1便!K6)</f>
         <v>東京支社　野村</v>
       </c>
-      <c r="L6" s="111"/>
+      <c r="L6" s="115"/>
       <c r="M6" s="41"/>
       <c r="N6" s="41"/>
     </row>
     <row r="7" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="112" t="str">
+      <c r="A7" s="116" t="str">
         <f>IF(情報!B2="","",情報!B2 &amp; "　壁")</f>
         <v>門沢橋3丁目2048番・B号棟　壁</v>
       </c>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="116"/>
+      <c r="L7" s="116"/>
       <c r="M7" s="40"/>
       <c r="N7" s="40"/>
     </row>
     <row r="8" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="108" t="s">
+      <c r="A8" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="109"/>
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
       <c r="G8" s="43"/>
@@ -4578,45 +4585,47 @@
       <c r="N16" s="41"/>
     </row>
     <row r="17" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="113" t="s">
+      <c r="A17" s="117" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="113"/>
-      <c r="C17" s="113"/>
-      <c r="D17" s="113"/>
-      <c r="E17" s="113"/>
-      <c r="F17" s="113"/>
-      <c r="G17" s="114">
+      <c r="B17" s="117"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="118">
         <v>1</v>
       </c>
-      <c r="H17" s="114"/>
-      <c r="I17" s="114"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="118"/>
       <c r="J17" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="115"/>
-      <c r="L17" s="115"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
       <c r="M17" s="41"/>
       <c r="N17" s="41"/>
     </row>
     <row r="18" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="109" t="s">
+      <c r="A18" s="113" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="109"/>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
-      <c r="G18" s="57">
-        <v>264</v>
-      </c>
-      <c r="H18" s="57">
-        <v>202</v>
+      <c r="B18" s="113"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="113"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="89" t="str">
+        <f>IF(情報!B14="","",情報!B14)</f>
+        <v/>
+      </c>
+      <c r="H18" s="89" t="str">
+        <f>IF(情報!C14="","",情報!C14)</f>
+        <v/>
       </c>
       <c r="I18" s="58">
         <f>SUM(G18:H18)</f>
-        <v>466</v>
+        <v>0</v>
       </c>
       <c r="J18" s="48" t="s">
         <v>89</v>
@@ -4630,14 +4639,14 @@
       <c r="N18" s="41"/>
     </row>
     <row r="19" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="116" t="s">
+      <c r="A19" s="110" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="116"/>
-      <c r="F19" s="116"/>
+      <c r="B19" s="110"/>
+      <c r="C19" s="110"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="110"/>
       <c r="G19" s="56"/>
       <c r="H19" s="61"/>
       <c r="I19" s="61">
@@ -4646,20 +4655,20 @@
       <c r="J19" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="K19" s="117"/>
-      <c r="L19" s="117"/>
+      <c r="K19" s="111"/>
+      <c r="L19" s="111"/>
       <c r="M19" s="41"/>
       <c r="N19" s="41"/>
     </row>
     <row r="20" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="116" t="s">
+      <c r="A20" s="110" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="116"/>
-      <c r="F20" s="116"/>
+      <c r="B20" s="110"/>
+      <c r="C20" s="110"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="110"/>
       <c r="G20" s="56"/>
       <c r="H20" s="61"/>
       <c r="I20" s="61">
@@ -4668,26 +4677,26 @@
       <c r="J20" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="K20" s="117"/>
-      <c r="L20" s="117"/>
+      <c r="K20" s="111"/>
+      <c r="L20" s="111"/>
       <c r="M20" s="41"/>
       <c r="N20" s="41"/>
     </row>
     <row r="21" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="118" t="s">
+      <c r="A21" s="112" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="118"/>
-      <c r="K21" s="118"/>
-      <c r="L21" s="118"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="112"/>
+      <c r="L21" s="112"/>
       <c r="M21" s="41"/>
       <c r="N21" s="41"/>
     </row>
@@ -4725,6 +4734,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="K17:L17"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="A1:L1"/>
@@ -4732,17 +4752,6 @@
     <mergeCell ref="A3:L3"/>
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="A21:L21"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update feedback 20190117 handle export excel and pdf
</commit_message>
<xml_diff>
--- a/public/template/Excel/template02.xlsx
+++ b/public/template/Excel/template02.xlsx
@@ -1,34 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\03\public\template\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB1C886-466A-4A12-85B2-E11D5D09C290}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="情報" sheetId="1" r:id="rId4"/>
-    <sheet name="工場1便" sheetId="2" r:id="rId5"/>
-    <sheet name="工場2便" sheetId="3" r:id="rId6"/>
-    <sheet name="工場3便" sheetId="4" r:id="rId7"/>
-    <sheet name="営業1便" sheetId="5" r:id="rId8"/>
-    <sheet name="営業2便" sheetId="6" r:id="rId9"/>
-    <sheet name="営業3便" sheetId="7" r:id="rId10"/>
+    <sheet name="情報" sheetId="1" r:id="rId1"/>
+    <sheet name="工場1便" sheetId="2" r:id="rId2"/>
+    <sheet name="工場2便" sheetId="3" r:id="rId3"/>
+    <sheet name="工場3便" sheetId="4" r:id="rId4"/>
+    <sheet name="営業1便" sheetId="5" r:id="rId5"/>
+    <sheet name="営業2便" sheetId="6" r:id="rId6"/>
+    <sheet name="営業3便" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'工場1便'!$A$1:$J$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'工場2便'!$A$1:$J$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'工場3便'!$A$1:$J$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'営業1便'!$A$1:$L$21</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'営業2便'!$A$1:$L$21</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'営業3便'!$A$1:$L$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">営業1便!$A$1:$L$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">営業2便!$A$1:$L$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">営業3便!$A$1:$L$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">工場1便!$A$1:$J$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">工場2便!$A$1:$J$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">工場3便!$A$1:$J$17</definedName>
   </definedNames>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="67">
   <si>
     <t>日付</t>
   </si>
@@ -100,54 +114,6 @@
   </si>
   <si>
     <t>依頼NO2</t>
-  </si>
-  <si>
-    <t>2018/11/13</t>
-  </si>
-  <si>
-    <t>門沢橋3丁目2048番・B号棟</t>
-  </si>
-  <si>
-    <t>紅中㈱　関東分</t>
-  </si>
-  <si>
-    <t>紅中㈱　多摩</t>
-  </si>
-  <si>
-    <t>㈱飯田産業</t>
-  </si>
-  <si>
-    <t>千葉</t>
-  </si>
-  <si>
-    <t>2018/11/21</t>
-  </si>
-  <si>
-    <t>2018/11/30</t>
-  </si>
-  <si>
-    <t>海老名市門沢橋３丁目２−２１</t>
-  </si>
-  <si>
-    <t>４ｔ</t>
-  </si>
-  <si>
-    <t>宮島裕和</t>
-  </si>
-  <si>
-    <t>東京都台東区寿3-14-11</t>
-  </si>
-  <si>
-    <t>03-6635-1650</t>
-  </si>
-  <si>
-    <t>03-5828-2860</t>
-  </si>
-  <si>
-    <t>東京支社</t>
-  </si>
-  <si>
-    <t>野村</t>
   </si>
   <si>
     <t>カットｍ</t>
@@ -283,63 +249,42 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00_ "/>
     <numFmt numFmtId="165" formatCode="[$-411]ggge&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
     <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Meiryo UI"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Meiryo UI"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Meiryo UI"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Meiryo UI"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="single"/>
+      <u/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Meiryo UI"/>
@@ -350,23 +295,31 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="13">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -376,6 +329,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -390,6 +344,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -401,6 +356,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -409,481 +366,412 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="100">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="37" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="164" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="37" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="164" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="37" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="164" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="37" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="8" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="9" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="10" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="true"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="14" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="11" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="165" fillId="2" borderId="11" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="165" fillId="2" borderId="12" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="166" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="38" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="37" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="37" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -895,7 +783,13 @@
     <xdr:ext cx="2085975" cy="266700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -907,7 +801,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="0"/>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -918,7 +815,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -930,7 +827,13 @@
     <xdr:ext cx="2085975" cy="266700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -942,7 +845,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="0"/>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -953,7 +859,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -965,7 +871,13 @@
     <xdr:ext cx="2085975" cy="266700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -977,7 +889,10 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="0"/>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -1274,46 +1189,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="true" style="14"/>
-    <col min="2" max="2" width="9" customWidth="true" style="0"/>
-    <col min="3" max="3" width="9" customWidth="true" style="0"/>
-    <col min="4" max="4" width="9" customWidth="true" style="0"/>
-    <col min="5" max="5" width="9" customWidth="true" style="0"/>
-    <col min="6" max="6" width="9" customWidth="true" style="0"/>
-    <col min="7" max="7" width="9" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9" customWidth="true" style="0"/>
-    <col min="9" max="9" width="9" customWidth="true" style="0"/>
-    <col min="10" max="10" width="9" customWidth="true" style="0"/>
-    <col min="11" max="11" width="9" customWidth="true" style="0"/>
-    <col min="12" max="12" width="9" customWidth="true" style="0"/>
-    <col min="13" max="13" width="9" customWidth="true" style="0"/>
-    <col min="14" max="14" width="9" customWidth="true" style="0"/>
-    <col min="15" max="15" width="9" customWidth="true" style="0"/>
-    <col min="16" max="16" width="9" customWidth="true" style="0"/>
-    <col min="17" max="17" width="9" customWidth="true" style="0"/>
-    <col min="18" max="18" width="9" customWidth="true" style="0"/>
-    <col min="19" max="19" width="9" customWidth="true" style="0"/>
-    <col min="20" max="20" width="9" customWidth="true" style="0"/>
-    <col min="21" max="21" width="9" customWidth="true" style="0"/>
-    <col min="22" max="22" width="9" customWidth="true" style="0"/>
-    <col min="23" max="23" width="9" customWidth="true" style="0"/>
-    <col min="24" max="24" width="9" customWidth="true" style="0"/>
+    <col min="1" max="1" width="9" style="14" customWidth="1"/>
+    <col min="2" max="24" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1387,152 +1277,91 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="14" t="s">
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="14">
-        <v>211850</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="B11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="14">
-        <v>211850</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="C11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="14">
-        <v>705360</v>
-      </c>
-      <c r="H2" s="14" t="s">
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="14" t="s">
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="14" t="s">
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" s="14">
-        <v>33</v>
-      </c>
-      <c r="X2" s="14">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24">
-      <c r="A10" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24">
-      <c r="A11" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24">
-      <c r="A12" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24">
-      <c r="A13" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
-      <c r="A14" s="14" t="s">
-        <v>46</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" scale="66" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" scale="66" orientation="landscape"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:J1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="true" defaultRowHeight="24.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="true" style="14"/>
-    <col min="2" max="2" width="15.5703125" customWidth="true" style="14"/>
-    <col min="3" max="3" width="6.140625" customWidth="true" style="14"/>
-    <col min="4" max="4" width="6.140625" customWidth="true" style="14"/>
-    <col min="5" max="5" width="6.140625" customWidth="true" style="14"/>
-    <col min="6" max="6" width="8.140625" customWidth="true" style="14"/>
-    <col min="7" max="7" width="6.140625" customWidth="true" style="14"/>
-    <col min="8" max="8" width="6.140625" customWidth="true" style="14"/>
-    <col min="9" max="9" width="6.140625" customWidth="true" style="14"/>
-    <col min="10" max="10" width="8.140625" customWidth="true" style="14"/>
-    <col min="11" max="11" width="9" customWidth="true" style="14"/>
-    <col min="12" max="12" width="9" customWidth="true" style="0"/>
+    <col min="1" max="1" width="8.5703125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="14" customWidth="1"/>
+    <col min="3" max="5" width="6.140625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="14" customWidth="1"/>
+    <col min="7" max="9" width="6.140625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="9" style="14" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" customHeight="1" ht="24.75">
+    <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="80" t="str">
         <f>IF(情報!A2="","",情報!A2)</f>
-        <v>2018/11/13</v>
+        <v/>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -1544,17 +1373,17 @@
       <c r="I1" s="80"/>
       <c r="J1" s="80"/>
     </row>
-    <row r="2" spans="1:12" customHeight="1" ht="24.75">
+    <row r="2" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="str">
         <f>IF(情報!K2="","",情報!K2&amp;"工場")</f>
-        <v>千葉工場</v>
+        <v/>
       </c>
       <c r="B2" s="81"/>
       <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" customHeight="1" ht="24.75">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
       <c r="B3" s="82"/>
       <c r="C3" s="82"/>
@@ -1566,7 +1395,7 @@
       <c r="I3" s="82"/>
       <c r="J3" s="82"/>
     </row>
-    <row r="4" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1580,9 +1409,9 @@
       <c r="I4" s="83"/>
       <c r="J4" s="84"/>
     </row>
-    <row r="5" spans="1:12" customHeight="1" ht="24.75">
+    <row r="5" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="85" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -1594,13 +1423,13 @@
       <c r="I5" s="85"/>
       <c r="J5" s="85"/>
     </row>
-    <row r="6" spans="1:12" customHeight="1" ht="24.75">
+    <row r="6" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="86" t="str">
         <f>IF(情報!B2="","",情報!B2&amp;"　先行壁")</f>
-        <v>門沢橋3丁目2048番・B号棟　先行壁</v>
+        <v/>
       </c>
       <c r="C6" s="87"/>
       <c r="D6" s="87"/>
@@ -1611,9 +1440,9 @@
       <c r="I6" s="87"/>
       <c r="J6" s="87"/>
     </row>
-    <row r="7" spans="1:12" customHeight="1" ht="24.75">
+    <row r="7" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B7" s="83"/>
       <c r="C7" s="87"/>
@@ -1625,13 +1454,13 @@
       <c r="I7" s="87"/>
       <c r="J7" s="87"/>
     </row>
-    <row r="8" spans="1:12" customHeight="1" ht="24.75">
+    <row r="8" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B8" s="88" t="str">
         <f>IF(情報!L2="","",情報!L2)</f>
-        <v>2018/11/21</v>
+        <v/>
       </c>
       <c r="C8" s="89"/>
       <c r="D8" s="89"/>
@@ -1642,13 +1471,13 @@
       <c r="I8" s="89"/>
       <c r="J8" s="89"/>
     </row>
-    <row r="9" spans="1:12" customHeight="1" ht="24.75">
+    <row r="9" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="86" t="str">
         <f>IF(情報!O2="","",情報!O2)</f>
-        <v>海老名市門沢橋３丁目２−２１</v>
+        <v/>
       </c>
       <c r="C9" s="87"/>
       <c r="D9" s="87"/>
@@ -1659,9 +1488,9 @@
       <c r="I9" s="87"/>
       <c r="J9" s="87"/>
     </row>
-    <row r="10" spans="1:12" customHeight="1" ht="24.75">
+    <row r="10" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="90" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B10" s="90"/>
       <c r="C10" s="90"/>
@@ -1673,52 +1502,52 @@
       <c r="I10" s="90"/>
       <c r="J10" s="90"/>
     </row>
-    <row r="11" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="H11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="J11" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="5" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -1727,25 +1556,25 @@
         <v>0</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" customHeight="1" ht="24.75">
+    <row r="13" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="66" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="44" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D13" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="66" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -1754,23 +1583,23 @@
         <v>0</v>
       </c>
       <c r="J13" s="48" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" customHeight="1" ht="24.75">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="66" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="44" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D14" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="66" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -1779,23 +1608,23 @@
         <v>0</v>
       </c>
       <c r="J14" s="48" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" customHeight="1" ht="24.75">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="66" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="44" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="66" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -1804,15 +1633,15 @@
         <v>0</v>
       </c>
       <c r="J15" s="48" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C16" s="75"/>
       <c r="D16" s="75"/>
@@ -1823,7 +1652,7 @@
       <c r="I16" s="75"/>
       <c r="J16" s="76"/>
     </row>
-    <row r="17" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="73"/>
       <c r="B17" s="77"/>
       <c r="C17" s="78"/>
@@ -1836,8 +1665,8 @@
       <c r="J17" s="79"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="12">
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:J17"/>
     <mergeCell ref="A1:J1"/>
@@ -1851,51 +1680,35 @@
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="A10:J10"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:J1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="true" defaultRowHeight="24.95" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="true" style="13"/>
-    <col min="2" max="2" width="15.5703125" customWidth="true" style="13"/>
-    <col min="3" max="3" width="6.140625" customWidth="true" style="13"/>
-    <col min="4" max="4" width="6.140625" customWidth="true" style="13"/>
-    <col min="5" max="5" width="6.140625" customWidth="true" style="13"/>
-    <col min="6" max="6" width="8.140625" customWidth="true" style="13"/>
-    <col min="7" max="7" width="6.140625" customWidth="true" style="13"/>
-    <col min="8" max="8" width="6.140625" customWidth="true" style="13"/>
-    <col min="9" max="9" width="6.140625" customWidth="true" style="13"/>
-    <col min="10" max="10" width="8.140625" customWidth="true" style="13"/>
-    <col min="11" max="11" width="9" customWidth="true" style="13"/>
-    <col min="12" max="12" width="9" customWidth="true" style="0"/>
+    <col min="1" max="1" width="8.5703125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="13" customWidth="1"/>
+    <col min="3" max="5" width="6.140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="13" customWidth="1"/>
+    <col min="7" max="9" width="6.140625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" style="13" customWidth="1"/>
+    <col min="11" max="11" width="9" style="13" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" customHeight="1" ht="24.75">
+    <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="80" t="str">
         <f>IF(工場1便!A1="","",工場1便!A1)</f>
-        <v>2018/11/13</v>
+        <v/>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -1907,17 +1720,17 @@
       <c r="I1" s="80"/>
       <c r="J1" s="80"/>
     </row>
-    <row r="2" spans="1:12" customHeight="1" ht="24.75">
+    <row r="2" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="str">
         <f>IF(工場1便!A2="","",工場1便!A2)</f>
-        <v>千葉工場</v>
+        <v/>
       </c>
       <c r="B2" s="81"/>
       <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" customHeight="1" ht="24.95">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
       <c r="B3" s="82"/>
       <c r="C3" s="82"/>
@@ -1929,7 +1742,7 @@
       <c r="I3" s="82"/>
       <c r="J3" s="82"/>
     </row>
-    <row r="4" spans="1:12" customHeight="1" ht="24.95">
+    <row r="4" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="63"/>
       <c r="B4" s="63"/>
       <c r="C4" s="63"/>
@@ -1946,9 +1759,9 @@
       </c>
       <c r="J4" s="84"/>
     </row>
-    <row r="5" spans="1:12" customHeight="1" ht="24.95">
+    <row r="5" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="85" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -1960,13 +1773,13 @@
       <c r="I5" s="85"/>
       <c r="J5" s="85"/>
     </row>
-    <row r="6" spans="1:12" customHeight="1" ht="24.95" s="3" customFormat="1">
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="86" t="str">
         <f>IF(情報!B2="","",情報!B2&amp;"　天井")</f>
-        <v>門沢橋3丁目2048番・B号棟　天井</v>
+        <v/>
       </c>
       <c r="C6" s="87"/>
       <c r="D6" s="87"/>
@@ -1977,9 +1790,9 @@
       <c r="I6" s="87"/>
       <c r="J6" s="87"/>
     </row>
-    <row r="7" spans="1:12" customHeight="1" ht="24.95" s="3" customFormat="1">
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B7" s="86" t="str">
         <f>IF(工場1便!B7="","",工場1便!B7)</f>
@@ -1995,13 +1808,13 @@
       <c r="J7" s="87"/>
       <c r="K7" s="15"/>
     </row>
-    <row r="8" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B8" s="86" t="str">
         <f>IF(情報!M2="","",情報!M2)</f>
-        <v>2018/11/30</v>
+        <v/>
       </c>
       <c r="C8" s="87"/>
       <c r="D8" s="87"/>
@@ -2012,13 +1825,13 @@
       <c r="I8" s="87"/>
       <c r="J8" s="87"/>
     </row>
-    <row r="9" spans="1:12" customHeight="1" ht="24.95" s="3" customFormat="1">
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="86" t="str">
         <f>IF(工場1便!B9="","",工場1便!B9)</f>
-        <v>海老名市門沢橋３丁目２−２１</v>
+        <v/>
       </c>
       <c r="C9" s="87"/>
       <c r="D9" s="87"/>
@@ -2029,9 +1842,9 @@
       <c r="I9" s="87"/>
       <c r="J9" s="87"/>
     </row>
-    <row r="10" spans="1:12" customHeight="1" ht="24.95" s="3" customFormat="1">
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="90" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B10" s="90"/>
       <c r="C10" s="90"/>
@@ -2043,52 +1856,52 @@
       <c r="I10" s="90"/>
       <c r="J10" s="90"/>
     </row>
-    <row r="11" spans="1:12" customHeight="1" ht="24.95" s="3" customFormat="1">
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="H11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="J11" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" customHeight="1" ht="24.95" s="3" customFormat="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="5" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -2097,25 +1910,25 @@
         <v>0</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" customHeight="1" ht="24" s="3" customFormat="1">
+    <row r="13" spans="1:12" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="5" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -2124,25 +1937,25 @@
         <v>0</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="14" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="65" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="44" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D14" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="65" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -2151,25 +1964,25 @@
         <v>0</v>
       </c>
       <c r="J14" s="48" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" customHeight="1" ht="27" s="3" customFormat="1">
+    <row r="15" spans="1:12" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="65" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="44" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="65" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -2178,17 +1991,17 @@
         <v>0</v>
       </c>
       <c r="J15" s="48" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" customHeight="1" ht="24.95" s="3" customFormat="1">
+    <row r="16" spans="1:12" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C16" s="75"/>
       <c r="D16" s="75"/>
@@ -2199,7 +2012,7 @@
       <c r="I16" s="75"/>
       <c r="J16" s="76"/>
     </row>
-    <row r="17" spans="1:12" customHeight="1" ht="24.95" s="3" customFormat="1">
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="73"/>
       <c r="B17" s="77"/>
       <c r="C17" s="78"/>
@@ -2212,8 +2025,8 @@
       <c r="J17" s="79"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="12">
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B9:J9"/>
@@ -2227,51 +2040,34 @@
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="I4:J4"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:J1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="true" defaultRowHeight="24.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="true" style="0"/>
-    <col min="2" max="2" width="15.5703125" customWidth="true" style="0"/>
-    <col min="3" max="3" width="6.140625" customWidth="true" style="0"/>
-    <col min="4" max="4" width="6.140625" customWidth="true" style="0"/>
-    <col min="5" max="5" width="6.140625" customWidth="true" style="0"/>
-    <col min="6" max="6" width="8.140625" customWidth="true" style="0"/>
-    <col min="7" max="7" width="6.140625" customWidth="true" style="0"/>
-    <col min="8" max="8" width="6.140625" customWidth="true" style="0"/>
-    <col min="9" max="9" width="6.140625" customWidth="true" style="0"/>
-    <col min="10" max="10" width="8.140625" customWidth="true" style="0"/>
-    <col min="11" max="11" width="9.140625" customWidth="true" style="0"/>
-    <col min="12" max="12" width="9.140625" customWidth="true" style="0"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="9" width="6.140625" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="80" t="str">
         <f>IF(工場1便!A1="","",工場1便!A1)</f>
-        <v>2018/11/13</v>
+        <v/>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -2283,14 +2079,14 @@
       <c r="I1" s="80"/>
       <c r="J1" s="80"/>
     </row>
-    <row r="2" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="str">
         <f>IF(工場1便!A2="","",工場1便!A2)</f>
-        <v>千葉工場</v>
+        <v/>
       </c>
       <c r="B2" s="81"/>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -2300,7 +2096,7 @@
       <c r="I2" s="17"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
       <c r="B3" s="82"/>
       <c r="C3" s="82"/>
@@ -2312,7 +2108,7 @@
       <c r="I3" s="82"/>
       <c r="J3" s="82"/>
     </row>
-    <row r="4" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2329,9 +2125,9 @@
       </c>
       <c r="J4" s="84"/>
     </row>
-    <row r="5" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="85" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B5" s="85"/>
       <c r="C5" s="85"/>
@@ -2343,13 +2139,13 @@
       <c r="I5" s="85"/>
       <c r="J5" s="85"/>
     </row>
-    <row r="6" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="86" t="str">
         <f>IF(情報!B2="","",情報!B2&amp;"　壁")</f>
-        <v>門沢橋3丁目2048番・B号棟　壁</v>
+        <v/>
       </c>
       <c r="C6" s="87"/>
       <c r="D6" s="87"/>
@@ -2360,9 +2156,9 @@
       <c r="I6" s="87"/>
       <c r="J6" s="87"/>
     </row>
-    <row r="7" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B7" s="86" t="str">
         <f>IF(工場1便!B7="","",工場1便!B7)</f>
@@ -2378,13 +2174,13 @@
       <c r="J7" s="87"/>
       <c r="K7" s="15"/>
     </row>
-    <row r="8" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B8" s="86" t="str">
         <f>IF(情報!N2="","",情報!N2)</f>
-        <v>2018/11/30</v>
+        <v/>
       </c>
       <c r="C8" s="87"/>
       <c r="D8" s="87"/>
@@ -2395,13 +2191,13 @@
       <c r="I8" s="87"/>
       <c r="J8" s="87"/>
     </row>
-    <row r="9" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="86" t="str">
         <f>IF(工場1便!B9="","",工場1便!B9)</f>
-        <v>海老名市門沢橋３丁目２−２１</v>
+        <v/>
       </c>
       <c r="C9" s="87"/>
       <c r="D9" s="87"/>
@@ -2412,9 +2208,9 @@
       <c r="I9" s="87"/>
       <c r="J9" s="87"/>
     </row>
-    <row r="10" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="90" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B10" s="90"/>
       <c r="C10" s="90"/>
@@ -2426,52 +2222,52 @@
       <c r="I10" s="90"/>
       <c r="J10" s="90"/>
     </row>
-    <row r="11" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="H11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="J11" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="5" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -2480,25 +2276,25 @@
         <v>0</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="13" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="5" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -2507,25 +2303,25 @@
         <v>0</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="14" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="5" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -2534,25 +2330,25 @@
         <v>0</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="15" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="65" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="44" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="65" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -2561,17 +2357,17 @@
         <v>0</v>
       </c>
       <c r="J15" s="48" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="16" spans="1:12" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C16" s="75"/>
       <c r="D16" s="75"/>
@@ -2582,7 +2378,7 @@
       <c r="I16" s="75"/>
       <c r="J16" s="76"/>
     </row>
-    <row r="17" spans="1:12" customHeight="1" ht="24.75" s="3" customFormat="1">
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="73"/>
       <c r="B17" s="77"/>
       <c r="C17" s="78"/>
@@ -2595,8 +2391,8 @@
       <c r="J17" s="79"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="12">
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B9:J9"/>
@@ -2610,48 +2406,30 @@
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="A5:J5"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:L1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="true" defaultRowHeight="24.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="true" style="0"/>
-    <col min="2" max="2" width="14.140625" customWidth="true" style="0"/>
-    <col min="3" max="3" width="5.5703125" customWidth="true" style="0"/>
-    <col min="4" max="4" width="5.5703125" customWidth="true" style="0"/>
-    <col min="5" max="5" width="5.5703125" customWidth="true" style="0"/>
-    <col min="6" max="6" width="8.140625" customWidth="true" style="0"/>
-    <col min="7" max="7" width="5.5703125" customWidth="true" style="0"/>
-    <col min="8" max="8" width="5.5703125" customWidth="true" style="0"/>
-    <col min="9" max="9" width="5.5703125" customWidth="true" style="0"/>
-    <col min="10" max="10" width="6.140625" customWidth="true" style="0"/>
-    <col min="11" max="11" width="6.140625" customWidth="true" style="0"/>
-    <col min="12" max="12" width="6.140625" customWidth="true" style="0"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="9" width="5.5703125" customWidth="1"/>
+    <col min="10" max="12" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" customHeight="1" ht="24.75">
+    <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="80"/>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -2665,7 +2443,7 @@
       <c r="K1" s="80"/>
       <c r="L1" s="80"/>
     </row>
-    <row r="2" spans="1:12" customHeight="1" ht="24.75">
+    <row r="2" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="82"/>
       <c r="B2" s="82"/>
       <c r="C2" s="82"/>
@@ -2679,10 +2457,10 @@
       <c r="K2" s="82"/>
       <c r="L2" s="82"/>
     </row>
-    <row r="3" spans="1:12" customHeight="1" ht="24.75">
+    <row r="3" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="80" t="str">
         <f>IF(情報!R2="","",情報!R2)</f>
-        <v>東京都台東区寿3-14-11</v>
+        <v/>
       </c>
       <c r="B3" s="80"/>
       <c r="C3" s="80"/>
@@ -2696,10 +2474,10 @@
       <c r="K3" s="80"/>
       <c r="L3" s="80"/>
     </row>
-    <row r="4" spans="1:12" customHeight="1" ht="24.75">
+    <row r="4" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="80" t="str">
         <f>IF(情報!S2="","","TEL "&amp;情報!S2)</f>
-        <v>TEL 03-6635-1650</v>
+        <v/>
       </c>
       <c r="B4" s="80"/>
       <c r="C4" s="80"/>
@@ -2713,10 +2491,10 @@
       <c r="K4" s="80"/>
       <c r="L4" s="80"/>
     </row>
-    <row r="5" spans="1:12" customHeight="1" ht="24.75">
+    <row r="5" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="80" t="str">
         <f>IF(情報!T2="","","FAX "&amp;情報!T2)</f>
-        <v>FAX 03-5828-2860</v>
+        <v/>
       </c>
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
@@ -2730,9 +2508,9 @@
       <c r="K5" s="80"/>
       <c r="L5" s="80"/>
     </row>
-    <row r="6" spans="1:12" customHeight="1" ht="24.75">
+    <row r="6" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="92" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B6" s="92"/>
       <c r="C6" s="69"/>
@@ -2748,10 +2526,10 @@
       <c r="K6" s="93"/>
       <c r="L6" s="83"/>
     </row>
-    <row r="7" spans="1:12" customHeight="1" ht="24.75">
+    <row r="7" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94" t="str">
         <f>IF(情報!B2="","",情報!B2&amp;"　先行壁")</f>
-        <v>門沢橋3丁目2048番・B号棟　先行壁</v>
+        <v/>
       </c>
       <c r="B7" s="94"/>
       <c r="C7" s="94"/>
@@ -2765,9 +2543,9 @@
       <c r="K7" s="94"/>
       <c r="L7" s="94"/>
     </row>
-    <row r="8" spans="1:12" customHeight="1" ht="24.75">
+    <row r="8" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="90" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -2781,231 +2559,231 @@
       <c r="K8" s="42"/>
       <c r="L8" s="52"/>
     </row>
-    <row r="9" spans="1:12" customHeight="1" ht="24.75">
+    <row r="9" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B9" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="J9" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="L9" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9" s="55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" customHeight="1" ht="24.75">
+    </row>
+    <row r="10" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="68" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B10" s="46"/>
       <c r="C10" s="44"/>
       <c r="D10" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E10" s="68"/>
       <c r="F10" s="68" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="G10" s="56"/>
       <c r="H10" s="71"/>
       <c r="I10" s="58">
-        <f>SUM(G10:H10)</f>
+        <f t="shared" ref="I10:I16" si="0">SUM(G10:H10)</f>
         <v>0</v>
       </c>
       <c r="J10" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K10" s="59"/>
       <c r="L10" s="71">
-        <f>SUM(I10*K10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" customHeight="1" ht="24.75">
+        <f t="shared" ref="L10:L16" si="1">SUM(I10*K10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="68" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B11" s="46"/>
       <c r="C11" s="44"/>
       <c r="D11" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E11" s="68"/>
       <c r="F11" s="68"/>
       <c r="G11" s="56"/>
       <c r="H11" s="71"/>
       <c r="I11" s="58">
-        <f>SUM(G11:H11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J11" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K11" s="59"/>
       <c r="L11" s="71">
-        <f>SUM(I11*K11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="68" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B12" s="46"/>
       <c r="C12" s="44"/>
       <c r="D12" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E12" s="68"/>
       <c r="F12" s="68"/>
       <c r="G12" s="71"/>
       <c r="H12" s="71"/>
       <c r="I12" s="58">
-        <f>SUM(G12:H12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J12" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K12" s="59"/>
       <c r="L12" s="71">
-        <f>SUM(I12*K12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="68" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B13" s="46"/>
       <c r="C13" s="44"/>
       <c r="D13" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E13" s="68"/>
       <c r="F13" s="68"/>
       <c r="G13" s="56"/>
       <c r="H13" s="71"/>
       <c r="I13" s="58">
-        <f>SUM(G13:H13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J13" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K13" s="59"/>
       <c r="L13" s="71">
-        <f>SUM(I13*K13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="68" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B14" s="46"/>
       <c r="C14" s="44"/>
       <c r="D14" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E14" s="68"/>
       <c r="F14" s="68"/>
       <c r="G14" s="71"/>
       <c r="H14" s="71"/>
       <c r="I14" s="58">
-        <f>SUM(G14:H14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J14" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K14" s="59"/>
       <c r="L14" s="71">
-        <f>SUM(I14*K14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="68" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B15" s="46"/>
       <c r="C15" s="44"/>
       <c r="D15" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E15" s="68"/>
       <c r="F15" s="68"/>
       <c r="G15" s="71"/>
       <c r="H15" s="71"/>
       <c r="I15" s="58">
-        <f>SUM(G15:H15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J15" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K15" s="59"/>
       <c r="L15" s="71">
-        <f>SUM(I15*K15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="68" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B16" s="46"/>
       <c r="C16" s="44"/>
       <c r="D16" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E16" s="68"/>
       <c r="F16" s="68"/>
       <c r="G16" s="71"/>
       <c r="H16" s="71"/>
       <c r="I16" s="58">
-        <f>SUM(G16:H16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J16" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K16" s="59"/>
       <c r="L16" s="71">
-        <f>SUM(I16*K16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="95" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B17" s="95"/>
       <c r="C17" s="95"/>
@@ -3018,14 +2796,14 @@
       <c r="H17" s="96"/>
       <c r="I17" s="96"/>
       <c r="J17" s="60" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="K17" s="97"/>
       <c r="L17" s="97"/>
     </row>
-    <row r="18" spans="1:12" customHeight="1" ht="24.75">
+    <row r="18" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="91" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B18" s="91"/>
       <c r="C18" s="91"/>
@@ -3045,7 +2823,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="48" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="K18" s="59"/>
       <c r="L18" s="71">
@@ -3053,9 +2831,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" customHeight="1" ht="24.75">
+    <row r="19" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="91" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B19" s="91"/>
       <c r="C19" s="91"/>
@@ -3068,14 +2846,14 @@
         <v>1</v>
       </c>
       <c r="J19" s="62" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="K19" s="98"/>
       <c r="L19" s="98"/>
     </row>
-    <row r="20" spans="1:12" customHeight="1" ht="24.75">
+    <row r="20" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="91" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B20" s="91"/>
       <c r="C20" s="91"/>
@@ -3088,14 +2866,14 @@
         <v>1</v>
       </c>
       <c r="J20" s="62" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="K20" s="98"/>
       <c r="L20" s="98"/>
     </row>
-    <row r="21" spans="1:12" customHeight="1" ht="24.75">
+    <row r="21" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="99" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B21" s="99"/>
       <c r="C21" s="99"/>
@@ -3110,8 +2888,8 @@
       <c r="L21" s="99"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="18">
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="A20:F20"/>
@@ -3131,50 +2909,32 @@
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="K17:L17"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:L1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="true" defaultRowHeight="24.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="true" style="13"/>
-    <col min="2" max="2" width="14.140625" customWidth="true" style="13"/>
-    <col min="3" max="3" width="5.5703125" customWidth="true" style="13"/>
-    <col min="4" max="4" width="5.5703125" customWidth="true" style="13"/>
-    <col min="5" max="5" width="5.5703125" customWidth="true" style="13"/>
-    <col min="6" max="6" width="8.140625" customWidth="true" style="13"/>
-    <col min="7" max="7" width="5.5703125" customWidth="true" style="13"/>
-    <col min="8" max="8" width="5.5703125" customWidth="true" style="13"/>
-    <col min="9" max="9" width="5.5703125" customWidth="true" style="13"/>
-    <col min="10" max="10" width="6.140625" customWidth="true" style="13"/>
-    <col min="11" max="11" width="6.140625" customWidth="true" style="13"/>
-    <col min="12" max="12" width="6.140625" customWidth="true" style="13"/>
-    <col min="13" max="13" width="9" customWidth="true" style="13"/>
+    <col min="1" max="1" width="4.5703125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="13" customWidth="1"/>
+    <col min="3" max="5" width="5.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="13" customWidth="1"/>
+    <col min="7" max="9" width="5.5703125" style="13" customWidth="1"/>
+    <col min="10" max="12" width="6.140625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="9" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" customHeight="1" ht="24.75">
+    <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="80"/>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -3188,7 +2948,7 @@
       <c r="K1" s="80"/>
       <c r="L1" s="80"/>
     </row>
-    <row r="2" spans="1:13" customHeight="1" ht="24.75">
+    <row r="2" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="82"/>
       <c r="B2" s="82"/>
       <c r="C2" s="82"/>
@@ -3202,10 +2962,10 @@
       <c r="K2" s="82"/>
       <c r="L2" s="82"/>
     </row>
-    <row r="3" spans="1:13" customHeight="1" ht="24.75">
+    <row r="3" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="80" t="str">
         <f>IF(営業1便!A3="","",営業1便!A3)</f>
-        <v>東京都台東区寿3-14-11</v>
+        <v/>
       </c>
       <c r="B3" s="80"/>
       <c r="C3" s="80"/>
@@ -3219,10 +2979,10 @@
       <c r="K3" s="80"/>
       <c r="L3" s="80"/>
     </row>
-    <row r="4" spans="1:13" customHeight="1" ht="24.75">
+    <row r="4" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="80" t="str">
         <f>IF(営業1便!A4="","",営業1便!A4)</f>
-        <v>TEL 03-6635-1650</v>
+        <v/>
       </c>
       <c r="B4" s="80"/>
       <c r="C4" s="80"/>
@@ -3236,10 +2996,10 @@
       <c r="K4" s="80"/>
       <c r="L4" s="80"/>
     </row>
-    <row r="5" spans="1:13" customHeight="1" ht="24.75">
+    <row r="5" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="80" t="str">
         <f>IF(営業1便!A5="","",営業1便!A5)</f>
-        <v>FAX 03-5828-2860</v>
+        <v/>
       </c>
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
@@ -3253,9 +3013,9 @@
       <c r="K5" s="80"/>
       <c r="L5" s="80"/>
     </row>
-    <row r="6" spans="1:13" customHeight="1" ht="24.75">
+    <row r="6" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="92" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B6" s="92"/>
       <c r="C6" s="50"/>
@@ -3274,10 +3034,10 @@
       </c>
       <c r="L6" s="83"/>
     </row>
-    <row r="7" spans="1:13" customHeight="1" ht="24.75">
+    <row r="7" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94" t="str">
         <f>IF(情報!B2="","",情報!B2&amp;"　天井")</f>
-        <v>門沢橋3丁目2048番・B号棟　天井</v>
+        <v/>
       </c>
       <c r="B7" s="94"/>
       <c r="C7" s="94"/>
@@ -3291,9 +3051,9 @@
       <c r="K7" s="94"/>
       <c r="L7" s="94"/>
     </row>
-    <row r="8" spans="1:13" customHeight="1" ht="24.75">
+    <row r="8" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="90" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -3307,233 +3067,233 @@
       <c r="K8" s="42"/>
       <c r="L8" s="52"/>
     </row>
-    <row r="9" spans="1:13" customHeight="1" ht="24.75">
+    <row r="9" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B9" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="J9" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="L9" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9" s="55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" customHeight="1" ht="24.75">
+    </row>
+    <row r="10" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B10" s="46"/>
       <c r="C10" s="44"/>
       <c r="D10" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E10" s="45"/>
       <c r="F10" s="64" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="G10" s="56"/>
       <c r="H10" s="57"/>
       <c r="I10" s="58">
-        <f>SUM(G10:H10)</f>
+        <f t="shared" ref="I10:I16" si="0">SUM(G10:H10)</f>
         <v>0</v>
       </c>
       <c r="J10" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K10" s="59"/>
       <c r="L10" s="57">
-        <f>SUM(I10*K10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" customHeight="1" ht="24.75">
+        <f t="shared" ref="L10:L16" si="1">SUM(I10*K10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B11" s="46"/>
       <c r="C11" s="44"/>
       <c r="D11" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E11" s="45"/>
       <c r="F11" s="64" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="G11" s="56"/>
       <c r="H11" s="57"/>
       <c r="I11" s="58">
-        <f>SUM(G11:H11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J11" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K11" s="59"/>
       <c r="L11" s="57">
-        <f>SUM(I11*K11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B12" s="46"/>
       <c r="C12" s="44"/>
       <c r="D12" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E12" s="45"/>
       <c r="F12" s="45"/>
       <c r="G12" s="57"/>
       <c r="H12" s="57"/>
       <c r="I12" s="58">
-        <f>SUM(G12:H12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J12" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K12" s="59"/>
       <c r="L12" s="57">
-        <f>SUM(I12*K12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B13" s="46"/>
       <c r="C13" s="44"/>
       <c r="D13" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E13" s="45"/>
       <c r="F13" s="45"/>
       <c r="G13" s="56"/>
       <c r="H13" s="57"/>
       <c r="I13" s="58">
-        <f>SUM(G13:H13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J13" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K13" s="59"/>
       <c r="L13" s="57">
-        <f>SUM(I13*K13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B14" s="46"/>
       <c r="C14" s="44"/>
       <c r="D14" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E14" s="45"/>
       <c r="F14" s="45"/>
       <c r="G14" s="57"/>
       <c r="H14" s="57"/>
       <c r="I14" s="58">
-        <f>SUM(G14:H14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J14" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K14" s="59"/>
       <c r="L14" s="57">
-        <f>SUM(I14*K14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B15" s="46"/>
       <c r="C15" s="44"/>
       <c r="D15" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E15" s="45"/>
       <c r="F15" s="45"/>
       <c r="G15" s="57"/>
       <c r="H15" s="57"/>
       <c r="I15" s="58">
-        <f>SUM(G15:H15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J15" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K15" s="59"/>
       <c r="L15" s="57">
-        <f>SUM(I15*K15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B16" s="46"/>
       <c r="C16" s="44"/>
       <c r="D16" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E16" s="45"/>
       <c r="F16" s="45"/>
       <c r="G16" s="57"/>
       <c r="H16" s="57"/>
       <c r="I16" s="58">
-        <f>SUM(G16:H16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J16" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K16" s="59"/>
       <c r="L16" s="57">
-        <f>SUM(I16*K16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" customHeight="1" ht="24.75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="95" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B17" s="95"/>
       <c r="C17" s="95"/>
@@ -3546,14 +3306,14 @@
       <c r="H17" s="96"/>
       <c r="I17" s="96"/>
       <c r="J17" s="60" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="K17" s="97"/>
       <c r="L17" s="97"/>
     </row>
-    <row r="18" spans="1:13" customHeight="1" ht="24.75">
+    <row r="18" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="91" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B18" s="91"/>
       <c r="C18" s="91"/>
@@ -3573,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="48" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="K18" s="59"/>
       <c r="L18" s="57">
@@ -3581,9 +3341,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" customHeight="1" ht="24.75">
+    <row r="19" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="91" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B19" s="91"/>
       <c r="C19" s="91"/>
@@ -3596,14 +3356,14 @@
         <v>1</v>
       </c>
       <c r="J19" s="62" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="K19" s="98"/>
       <c r="L19" s="98"/>
     </row>
-    <row r="20" spans="1:13" customHeight="1" ht="24.75">
+    <row r="20" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="91" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B20" s="91"/>
       <c r="C20" s="91"/>
@@ -3616,14 +3376,14 @@
         <v>1</v>
       </c>
       <c r="J20" s="62" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="K20" s="98"/>
       <c r="L20" s="98"/>
     </row>
-    <row r="21" spans="1:13" customHeight="1" ht="24.75">
+    <row r="21" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="99" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B21" s="99"/>
       <c r="C21" s="99"/>
@@ -3638,8 +3398,8 @@
       <c r="L21" s="99"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="18">
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="K6:L6"/>
@@ -3659,51 +3419,32 @@
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="A5:L5"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:L1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="true" defaultRowHeight="24.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="true" style="0"/>
-    <col min="2" max="2" width="14.140625" customWidth="true" style="0"/>
-    <col min="3" max="3" width="5.5703125" customWidth="true" style="0"/>
-    <col min="4" max="4" width="5.5703125" customWidth="true" style="0"/>
-    <col min="5" max="5" width="5.5703125" customWidth="true" style="0"/>
-    <col min="6" max="6" width="8.140625" customWidth="true" style="0"/>
-    <col min="7" max="7" width="5.5703125" customWidth="true" style="0"/>
-    <col min="8" max="8" width="5.5703125" customWidth="true" style="0"/>
-    <col min="9" max="9" width="5.5703125" customWidth="true" style="0"/>
-    <col min="10" max="10" width="6.140625" customWidth="true" style="0"/>
-    <col min="11" max="11" width="6.140625" customWidth="true" style="0"/>
-    <col min="12" max="12" width="6.140625" customWidth="true" style="0"/>
-    <col min="13" max="13" width="9.140625" customWidth="true" style="0"/>
-    <col min="14" max="14" width="9.140625" customWidth="true" style="0"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="9" width="5.5703125" customWidth="1"/>
+    <col min="10" max="12" width="6.140625" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" customHeight="1" ht="24.75">
+    <row r="1" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="80"/>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
@@ -3719,7 +3460,7 @@
       <c r="M1" s="18"/>
       <c r="N1" s="18"/>
     </row>
-    <row r="2" spans="1:14" customHeight="1" ht="24.75">
+    <row r="2" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="82"/>
       <c r="B2" s="82"/>
       <c r="C2" s="82"/>
@@ -3735,10 +3476,10 @@
       <c r="M2" s="20"/>
       <c r="N2" s="20"/>
     </row>
-    <row r="3" spans="1:14" customHeight="1" ht="24.75">
+    <row r="3" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="80" t="str">
         <f>IF(営業1便!A3="","",営業1便!A3)</f>
-        <v>東京都台東区寿3-14-11</v>
+        <v/>
       </c>
       <c r="B3" s="80"/>
       <c r="C3" s="80"/>
@@ -3754,10 +3495,10 @@
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
     </row>
-    <row r="4" spans="1:14" customHeight="1" ht="24.75">
+    <row r="4" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="80" t="str">
         <f>IF(営業1便!A4="","",営業1便!A4)</f>
-        <v>TEL 03-6635-1650</v>
+        <v/>
       </c>
       <c r="B4" s="80"/>
       <c r="C4" s="80"/>
@@ -3773,10 +3514,10 @@
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
     </row>
-    <row r="5" spans="1:14" customHeight="1" ht="24.75">
+    <row r="5" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="80" t="str">
         <f>IF(営業1便!A5="","",営業1便!A5)</f>
-        <v>FAX 03-5828-2860</v>
+        <v/>
       </c>
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
@@ -3792,9 +3533,9 @@
       <c r="M5" s="18"/>
       <c r="N5" s="18"/>
     </row>
-    <row r="6" spans="1:14" customHeight="1" ht="24.75">
+    <row r="6" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="92" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B6" s="92"/>
       <c r="C6" s="29"/>
@@ -3815,10 +3556,10 @@
       <c r="M6" s="20"/>
       <c r="N6" s="20"/>
     </row>
-    <row r="7" spans="1:14" customHeight="1" ht="24.75">
+    <row r="7" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="94" t="str">
         <f>IF(情報!B2="","",情報!B2&amp;"　壁")</f>
-        <v>門沢橋3丁目2048番・B号棟　壁</v>
+        <v/>
       </c>
       <c r="B7" s="94"/>
       <c r="C7" s="94"/>
@@ -3834,9 +3575,9 @@
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
     </row>
-    <row r="8" spans="1:14" customHeight="1" ht="24.75">
+    <row r="8" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="90" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
@@ -3852,251 +3593,251 @@
       <c r="M8" s="19"/>
       <c r="N8" s="19"/>
     </row>
-    <row r="9" spans="1:14" customHeight="1" ht="24.75">
+    <row r="9" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B9" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="J9" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="L9" s="34" t="s">
         <v>55</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9" s="34" t="s">
-        <v>71</v>
       </c>
       <c r="M9" s="20"/>
       <c r="N9" s="20"/>
     </row>
-    <row r="10" spans="1:14" customHeight="1" ht="24.75">
+    <row r="10" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="23"/>
       <c r="D10" s="26" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="65" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="G10" s="35"/>
       <c r="H10" s="36"/>
       <c r="I10" s="37">
-        <f>SUM(G10:H10)</f>
+        <f t="shared" ref="I10:I16" si="0">SUM(G10:H10)</f>
         <v>0</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K10" s="38"/>
       <c r="L10" s="36">
-        <f>SUM(I10*K10)</f>
+        <f t="shared" ref="L10:L16" si="1">SUM(I10*K10)</f>
         <v>0</v>
       </c>
       <c r="M10" s="20"/>
       <c r="N10" s="20"/>
     </row>
-    <row r="11" spans="1:14" customHeight="1" ht="24.75">
+    <row r="11" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="23"/>
       <c r="D11" s="26" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="65" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="G11" s="35"/>
       <c r="H11" s="36"/>
       <c r="I11" s="58">
-        <f>SUM(G11:H11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K11" s="38"/>
       <c r="L11" s="57">
-        <f>SUM(I11*K11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M11" s="20"/>
       <c r="N11" s="20"/>
     </row>
-    <row r="12" spans="1:14" customHeight="1" ht="24.75">
+    <row r="12" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="23"/>
       <c r="D12" s="26" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="65" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="G12" s="36"/>
       <c r="H12" s="36"/>
       <c r="I12" s="58">
-        <f>SUM(G12:H12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K12" s="38"/>
       <c r="L12" s="57">
-        <f>SUM(I12*K12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M12" s="20"/>
       <c r="N12" s="20"/>
     </row>
-    <row r="13" spans="1:14" customHeight="1" ht="24.75">
+    <row r="13" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="23"/>
       <c r="D13" s="26" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
       <c r="G13" s="35"/>
       <c r="H13" s="36"/>
       <c r="I13" s="58">
-        <f>SUM(G13:H13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K13" s="38"/>
       <c r="L13" s="57">
-        <f>SUM(I13*K13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M13" s="20"/>
       <c r="N13" s="20"/>
     </row>
-    <row r="14" spans="1:14" customHeight="1" ht="24.75">
+    <row r="14" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="23"/>
       <c r="D14" s="26" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
       <c r="I14" s="58">
-        <f>SUM(G14:H14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K14" s="38"/>
       <c r="L14" s="57">
-        <f>SUM(I14*K14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M14" s="20"/>
       <c r="N14" s="20"/>
     </row>
-    <row r="15" spans="1:14" customHeight="1" ht="24.75">
+    <row r="15" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="23"/>
       <c r="D15" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
       <c r="I15" s="58">
-        <f>SUM(G15:H15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J15" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K15" s="38"/>
       <c r="L15" s="57">
-        <f>SUM(I15*K15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M15" s="20"/>
       <c r="N15" s="20"/>
     </row>
-    <row r="16" spans="1:14" customHeight="1" ht="24.75">
+    <row r="16" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B16" s="25"/>
       <c r="C16" s="23"/>
       <c r="D16" s="47" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
       <c r="I16" s="58">
-        <f>SUM(G16:H16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J16" s="48" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="K16" s="38"/>
       <c r="L16" s="57">
-        <f>SUM(I16*K16)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
     </row>
-    <row r="17" spans="1:14" customHeight="1" ht="24.75">
+    <row r="17" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="95" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B17" s="95"/>
       <c r="C17" s="95"/>
@@ -4109,16 +3850,16 @@
       <c r="H17" s="96"/>
       <c r="I17" s="96"/>
       <c r="J17" s="39" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="K17" s="97"/>
       <c r="L17" s="97"/>
       <c r="M17" s="20"/>
       <c r="N17" s="20"/>
     </row>
-    <row r="18" spans="1:14" customHeight="1" ht="24.75">
+    <row r="18" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="91" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B18" s="91"/>
       <c r="C18" s="91"/>
@@ -4138,7 +3879,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="K18" s="38"/>
       <c r="L18" s="36">
@@ -4148,9 +3889,9 @@
       <c r="M18" s="20"/>
       <c r="N18" s="20"/>
     </row>
-    <row r="19" spans="1:14" customHeight="1" ht="24.75">
+    <row r="19" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="91" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B19" s="91"/>
       <c r="C19" s="91"/>
@@ -4163,16 +3904,16 @@
         <v>1</v>
       </c>
       <c r="J19" s="41" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="K19" s="98"/>
       <c r="L19" s="98"/>
       <c r="M19" s="20"/>
       <c r="N19" s="20"/>
     </row>
-    <row r="20" spans="1:14" customHeight="1" ht="24.75">
+    <row r="20" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="91" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B20" s="91"/>
       <c r="C20" s="91"/>
@@ -4185,16 +3926,16 @@
         <v>1</v>
       </c>
       <c r="J20" s="41" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="K20" s="98"/>
       <c r="L20" s="98"/>
       <c r="M20" s="20"/>
       <c r="N20" s="20"/>
     </row>
-    <row r="21" spans="1:14" customHeight="1" ht="24.75">
+    <row r="21" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="99" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B21" s="99"/>
       <c r="C21" s="99"/>
@@ -4210,7 +3951,7 @@
       <c r="M21" s="20"/>
       <c r="N21" s="20"/>
     </row>
-    <row r="22" spans="1:14" customHeight="1" ht="24.75">
+    <row r="22" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -4226,7 +3967,7 @@
       <c r="M22" s="20"/>
       <c r="N22" s="20"/>
     </row>
-    <row r="23" spans="1:14" customHeight="1" ht="24.75">
+    <row r="23" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
@@ -4243,8 +3984,8 @@
       <c r="N23" s="20"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="18">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="A1:L1"/>
@@ -4264,17 +4005,8 @@
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="A21:L21"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>